<commit_message>
Mise à jour du suivi_projet
Ajout des tâches réalisées hier après-midi
</commit_message>
<xml_diff>
--- a/Gestion projet/suivi_projet.xlsx
+++ b/Gestion projet/suivi_projet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A80BEA-9661-4EAF-8D39-B4AC952915B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D26609-0C4B-4AC7-BAEE-78C399A15BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
+    <workbookView xWindow="-1335" yWindow="3300" windowWidth="21600" windowHeight="11385" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Lecture de la documentation de l'afficheur à LED défilant Mc Crypt n°590996</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>https://www.eztcp.com/en/download/pds_files/cseh53nen.pdf</t>
+  </si>
+  <si>
+    <t>Mettre en ordre le dépôt GIT et avec ça la création d'un README</t>
+  </si>
+  <si>
+    <t>Création d'un diagramme de cas d'utilisation en rapport avec le projet</t>
+  </si>
+  <si>
+    <t>Création d'un shéma réseau en rapport avec le projet</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -146,8 +158,8 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -484,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4521D194-E84C-4CFA-9C75-1EDA66349D08}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +509,7 @@
     <col min="4" max="4" width="62" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
@@ -508,20 +520,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>45803</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,9 +541,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -539,9 +551,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="9"/>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
@@ -549,165 +563,186 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>45804</v>
       </c>
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>45805</v>
       </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>45806</v>
       </c>
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>45807</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>45808</v>
       </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>45809</v>
       </c>
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>45810</v>
       </c>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>45811</v>
-      </c>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>45812</v>
-      </c>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>45813</v>
-      </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>45814</v>
       </c>
       <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>45815</v>
+        <v>45812</v>
       </c>
       <c r="B17" s="8"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>45816</v>
+        <v>45813</v>
       </c>
       <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>45817</v>
+        <v>45814</v>
       </c>
       <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>45818</v>
+        <v>45815</v>
       </c>
       <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>45819</v>
+        <v>45816</v>
       </c>
       <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>45820</v>
+        <v>45817</v>
       </c>
       <c r="B22" s="8"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>45821</v>
+        <v>45818</v>
       </c>
       <c r="B23" s="8"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>45822</v>
+        <v>45819</v>
       </c>
       <c r="B24" s="8"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>45823</v>
+        <v>45820</v>
       </c>
       <c r="B25" s="8"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>45824</v>
+        <v>45821</v>
       </c>
       <c r="B26" s="8"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>45825</v>
+        <v>45822</v>
       </c>
       <c r="B27" s="8"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>45826</v>
+        <v>45823</v>
       </c>
       <c r="B28" s="8"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>45827</v>
+        <v>45824</v>
       </c>
       <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
+        <v>45825</v>
+      </c>
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>45826</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>45827</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
         <v>45828</v>
       </c>
-      <c r="B30" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
+  <mergeCells count="3">
     <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{DF417EC4-481B-4F4B-81E5-B6626A4923F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Création fichiers et dossier
Nouveau dossier IHM dans Projet contenant des images et explication en détail de l'IHM
</commit_message>
<xml_diff>
--- a/Gestion projet/suivi_projet.xlsx
+++ b/Gestion projet/suivi_projet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D26609-0C4B-4AC7-BAEE-78C399A15BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1CFAD2-CF4B-49F8-B7E2-43F2B39BD852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1335" yWindow="3300" windowWidth="21600" windowHeight="11385" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
+    <workbookView xWindow="2715" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Lecture de la documentation de l'afficheur à LED défilant Mc Crypt n°590996</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>4h</t>
+  </si>
+  <si>
+    <t>Réflexion, conceptualisation et explication de l'IHM de l'application</t>
   </si>
 </sst>
 </file>
@@ -133,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -154,12 +157,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -499,18 +507,19 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="5"/>
+    <col min="1" max="2" width="11.42578125" style="9"/>
     <col min="3" max="3" width="34" style="1" customWidth="1"/>
     <col min="4" max="4" width="62" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -521,10 +530,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="10">
         <v>45803</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -532,8 +541,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,8 +551,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -552,8 +561,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -564,172 +573,177 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>45804</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="11">
         <v>45805</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="11">
         <v>45806</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="11">
         <v>45807</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="11">
         <v>45808</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="11">
         <v>45809</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="11">
         <v>45810</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="11">
         <v>45811</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="11">
         <v>45812</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="11">
         <v>45813</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="11"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="11">
         <v>45814</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="11">
         <v>45815</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="11">
         <v>45816</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="11"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="11">
         <v>45817</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="11"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="11">
         <v>45818</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="11"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="11">
         <v>45819</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="A25" s="11">
         <v>45820</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="11"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="11">
         <v>45821</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="11"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="11">
         <v>45822</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="11">
         <v>45823</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="11">
         <v>45824</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="11"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="11">
         <v>45825</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="11"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="11">
         <v>45826</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="11">
         <v>45827</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="11">
         <v>45828</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modif Application & Gestion
- suivi_projet
- Ajout stylesheet
- Modif MainWindow
</commit_message>
<xml_diff>
--- a/Gestion projet/suivi_projet.xlsx
+++ b/Gestion projet/suivi_projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B0AC04-0FA9-4066-B568-A8C3A9030632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B6ABDC-E4D5-4D18-811C-40556642F852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Lecture de la documentation de l'afficheur à LED défilant Mc Crypt n°590996</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Réglage de l'interface + essayer de corriger bug modification</t>
+  </si>
+  <si>
+    <t>Essayer corriger bug modification</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1043,12 @@
       <c r="A44" s="10">
         <v>45820</v>
       </c>
-      <c r="B44" s="10"/>
+      <c r="B44" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="10">

</xml_diff>

<commit_message>
Guide installation + suivi_projet
</commit_message>
<xml_diff>
--- a/Gestion projet/suivi_projet.xlsx
+++ b/Gestion projet/suivi_projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B6ABDC-E4D5-4D18-811C-40556642F852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025D99C9-159F-40D1-87BF-ECA3FB2B9D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>Lecture de la documentation de l'afficheur à LED défilant Mc Crypt n°590996</t>
   </si>
@@ -189,6 +189,21 @@
   </si>
   <si>
     <t>Essayer corriger bug modification</t>
+  </si>
+  <si>
+    <t>Correction bug modification + Mise au point</t>
+  </si>
+  <si>
+    <t>Réflexion amélioration de l'interface</t>
+  </si>
+  <si>
+    <t>Intégration d'ouverture d'un PDF</t>
+  </si>
+  <si>
+    <t>Début d'amélioration de l'interface</t>
+  </si>
+  <si>
+    <t>Écriture et intégration d'images au guide d'installation</t>
   </si>
 </sst>
 </file>
@@ -631,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4521D194-E84C-4CFA-9C75-1EDA66349D08}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,52 +1065,90 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
         <v>45821</v>
       </c>
-      <c r="B45" s="10"/>
+      <c r="B45" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+      <c r="A46" s="12"/>
+      <c r="B46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
         <v>45822</v>
       </c>
-      <c r="B46" s="10"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="B49" s="10"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
         <v>45823</v>
       </c>
-      <c r="B47" s="10"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
+      <c r="B50" s="10"/>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
         <v>45824</v>
       </c>
-      <c r="B48" s="10"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
+      <c r="B51" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
         <v>45825</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
         <v>45826</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
         <v>45827</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="10">
         <v>45828</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A45:A48"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="B2:B4"/>
@@ -1109,7 +1162,7 @@
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A18:A19"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:A9 A12 A17:A18 A20:A22 A27 A29 A31 A35:A39 A42 A44:A1048576">
+  <conditionalFormatting sqref="A1:A9 A12 A17:A18 A20:A22 A27 A29 A31 A35:A39 A42 A44:A45 A49:A1048576">
     <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today">
       <formula>FLOOR(A1,1)=TODAY()</formula>
     </cfRule>

</xml_diff>

<commit_message>
maj suivi_projet + application
</commit_message>
<xml_diff>
--- a/Gestion projet/suivi_projet.xlsx
+++ b/Gestion projet/suivi_projet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Stage\Stage_2025_ST_felixDL\Gestion projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitHub\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C516A667-55BD-469D-8CB4-CFF10A2DC513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA6AA09-4CF1-487C-9BD5-6BDF7C996358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Lecture de la documentation de l'afficheur à LED défilant Mc Crypt n°590996</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>6h</t>
+  </si>
+  <si>
+    <t>Fin d'écriture du guide d'installation</t>
+  </si>
+  <si>
+    <t>Crash test application et réglage de bugs</t>
+  </si>
+  <si>
+    <t>Réorganisation interface + optimisation de l'utilisation de la gestion d'indices</t>
   </si>
 </sst>
 </file>
@@ -295,11 +304,11 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -652,7 +661,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,10 +684,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="13">
         <v>45803</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -686,8 +695,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,8 +705,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -706,8 +715,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -718,8 +727,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
@@ -727,21 +736,21 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <v>45804</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -752,7 +761,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
@@ -761,7 +770,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
@@ -770,7 +779,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>45805</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -781,7 +790,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
@@ -790,7 +799,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="10" t="s">
         <v>19</v>
       </c>
@@ -799,7 +808,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="10" t="s">
         <v>17</v>
       </c>
@@ -808,7 +817,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="10" t="s">
         <v>17</v>
       </c>
@@ -823,7 +832,7 @@
       <c r="B17" s="10"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>45807</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -834,7 +843,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="10" t="s">
         <v>19</v>
       </c>
@@ -855,7 +864,7 @@
       <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="13">
         <v>45810</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -866,7 +875,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="10" t="s">
         <v>29</v>
       </c>
@@ -875,7 +884,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="10" t="s">
         <v>19</v>
       </c>
@@ -884,7 +893,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="10" t="s">
         <v>17</v>
       </c>
@@ -893,7 +902,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="10" t="s">
         <v>17</v>
       </c>
@@ -902,7 +911,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="13">
         <v>45811</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -913,7 +922,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
@@ -922,7 +931,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
+      <c r="A29" s="13">
         <v>45812</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -933,7 +942,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="10" t="s">
         <v>9</v>
       </c>
@@ -942,7 +951,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="A31" s="13">
         <v>45813</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -953,7 +962,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="10" t="s">
         <v>17</v>
       </c>
@@ -962,7 +971,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="10" t="s">
         <v>17</v>
       </c>
@@ -971,7 +980,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="10" t="s">
         <v>19</v>
       </c>
@@ -1009,7 +1018,7 @@
       <c r="B38" s="10"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
+      <c r="A39" s="13">
         <v>45818</v>
       </c>
       <c r="B39" s="10" t="s">
@@ -1020,7 +1029,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="10" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1038,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="10" t="s">
         <v>14</v>
       </c>
@@ -1038,20 +1047,20 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
+      <c r="A42" s="13">
         <v>45819</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="13"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
@@ -1065,7 +1074,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="12">
+      <c r="A45" s="13">
         <v>45821</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -1076,7 +1085,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="10" t="s">
         <v>9</v>
       </c>
@@ -1085,7 +1094,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="10" t="s">
         <v>17</v>
       </c>
@@ -1094,7 +1103,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="10" t="s">
         <v>19</v>
       </c>
@@ -1129,15 +1138,33 @@
       <c r="A52" s="10">
         <v>45825</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>45826</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>45827</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>